<commit_message>
BAP raporu Ek-3 haricinde bitti.
</commit_message>
<xml_diff>
--- a/IMMD BAP/bütçe-update.xlsx
+++ b/IMMD BAP/bütçe-update.xlsx
@@ -566,7 +566,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="A19" sqref="A19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="L4" s="11">
         <f>H19</f>
-        <v>3717</v>
+        <v>5097.5999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -761,19 +761,19 @@
         <v>25</v>
       </c>
       <c r="D7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="1"/>
-        <v>472</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>34</v>
@@ -784,7 +784,7 @@
       </c>
       <c r="L7" s="11">
         <f>SUM(L4:L6)</f>
-        <v>16225</v>
+        <v>17605.599999999999</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -802,16 +802,15 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5">
-        <f t="shared" ref="F8:F17" si="2">3.5*1.3*E8</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H8" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1770</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>31</v>
@@ -862,15 +861,15 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="1"/>
-        <v>177</v>
+        <v>212.39999999999998</v>
       </c>
       <c r="I10" s="10"/>
     </row>
@@ -970,15 +969,15 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="1"/>
-        <v>236</v>
+        <v>283.2</v>
       </c>
       <c r="I14" s="10"/>
     </row>
@@ -997,7 +996,7 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="0"/>
@@ -1020,11 +1019,11 @@
         <v>25</v>
       </c>
       <c r="D16" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F8:F17" si="2">3.5*1.3*E16</f>
         <v>0</v>
       </c>
       <c r="G16" s="8">
@@ -1050,7 +1049,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5">
@@ -1108,7 +1107,7 @@
       <c r="G19" s="17"/>
       <c r="H19" s="8">
         <f>SUM(H7:H18)</f>
-        <v>3717</v>
+        <v>5097.5999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>